<commit_message>
Added summary tables and updated cleaned data
</commit_message>
<xml_diff>
--- a/MsiaAccidentCasesTrain.xlsx
+++ b/MsiaAccidentCasesTrain.xlsx
@@ -57,13 +57,13 @@
     <t>A series of avalanche trapped victim who was mining prior to the incident</t>
   </si>
   <si>
+    <t>Died being run over by a lorry</t>
+  </si>
+  <si>
+    <t>Accident involving an employee who has been run over by a lorry while riding his motorcycle</t>
+  </si>
+  <si>
     <t>Fires and Explosion</t>
-  </si>
-  <si>
-    <t>Died being run over by a lorry</t>
-  </si>
-  <si>
-    <t>Accident involving an employee who has been run over by a lorry while riding his motorcycle</t>
   </si>
   <si>
     <t>Died due to explosion of boiler</t>
@@ -1173,7 +1173,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="10"/>
+        <fgColor indexed="9"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -1188,11 +1188,11 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -1201,7 +1201,7 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -1209,65 +1209,65 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1281,7 +1281,7 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top/>
       <bottom/>
@@ -1289,10 +1289,10 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top/>
       <bottom/>
@@ -1304,53 +1304,50 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -1376,8 +1373,8 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ffffffff"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1576,17 +1573,17 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1614,10 +1611,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1865,12 +1862,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -2157,7 +2154,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -2185,10 +2182,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -2520,20 +2517,20 @@
     </row>
     <row r="6" ht="15" customHeight="1">
       <c r="A6" t="s" s="8">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s" s="8">
         <v>14</v>
       </c>
-      <c r="B6" t="s" s="8">
+      <c r="C6" t="s" s="8">
         <v>15</v>
-      </c>
-      <c r="C6" t="s" s="8">
-        <v>16</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
     </row>
     <row r="7" ht="15" customHeight="1">
       <c r="A7" t="s" s="8">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s" s="8">
         <v>17</v>
@@ -2598,7 +2595,7 @@
     </row>
     <row r="12" ht="15" customHeight="1">
       <c r="A12" t="s" s="8">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s" s="8">
         <v>29</v>
@@ -2688,30 +2685,30 @@
       <c r="E18" s="10"/>
     </row>
     <row r="19" ht="15" customHeight="1">
-      <c r="A19" t="s" s="11">
+      <c r="A19" t="s" s="8">
         <v>22</v>
       </c>
-      <c r="B19" t="s" s="11">
+      <c r="B19" t="s" s="8">
         <v>41</v>
       </c>
-      <c r="C19" t="s" s="12">
+      <c r="C19" t="s" s="11">
         <v>42</v>
       </c>
-      <c r="D19" s="13"/>
-      <c r="E19" s="14"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="13"/>
     </row>
     <row r="20" ht="15" customHeight="1">
-      <c r="A20" t="s" s="11">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s" s="11">
+      <c r="A20" t="s" s="8">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s" s="8">
         <v>34</v>
       </c>
-      <c r="C20" t="s" s="12">
+      <c r="C20" t="s" s="11">
         <v>43</v>
       </c>
-      <c r="D20" s="13"/>
-      <c r="E20" s="14"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="13"/>
     </row>
     <row r="21" ht="15" customHeight="1">
       <c r="A21" t="s" s="8">
@@ -2723,21 +2720,21 @@
       <c r="C21" t="s" s="8">
         <v>44</v>
       </c>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
     </row>
     <row r="22" ht="15" customHeight="1">
-      <c r="A22" t="s" s="11">
+      <c r="A22" t="s" s="8">
         <v>22</v>
       </c>
-      <c r="B22" t="s" s="11">
+      <c r="B22" t="s" s="8">
         <v>41</v>
       </c>
-      <c r="C22" t="s" s="12">
+      <c r="C22" t="s" s="11">
         <v>45</v>
       </c>
-      <c r="D22" s="13"/>
-      <c r="E22" s="14"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="13"/>
     </row>
     <row r="23" ht="15" customHeight="1">
       <c r="A23" t="s" s="8">
@@ -2896,17 +2893,17 @@
       <c r="E34" s="10"/>
     </row>
     <row r="35" ht="15" customHeight="1">
-      <c r="A35" t="s" s="11">
+      <c r="A35" t="s" s="8">
         <v>9</v>
       </c>
-      <c r="B35" t="s" s="11">
+      <c r="B35" t="s" s="8">
         <v>66</v>
       </c>
-      <c r="C35" t="s" s="12">
+      <c r="C35" t="s" s="11">
         <v>67</v>
       </c>
-      <c r="D35" s="13"/>
-      <c r="E35" s="14"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="13"/>
     </row>
     <row r="36" ht="15" customHeight="1">
       <c r="A36" t="s" s="8">
@@ -3104,17 +3101,17 @@
       <c r="E50" s="10"/>
     </row>
     <row r="51" ht="15" customHeight="1">
-      <c r="A51" t="s" s="11">
+      <c r="A51" t="s" s="8">
         <v>3</v>
       </c>
-      <c r="B51" t="s" s="11">
+      <c r="B51" t="s" s="8">
         <v>94</v>
       </c>
-      <c r="C51" t="s" s="12">
+      <c r="C51" t="s" s="11">
         <v>95</v>
       </c>
-      <c r="D51" s="13"/>
-      <c r="E51" s="14"/>
+      <c r="D51" s="12"/>
+      <c r="E51" s="13"/>
     </row>
     <row r="52" ht="15" customHeight="1">
       <c r="A52" t="s" s="8">
@@ -3126,21 +3123,21 @@
       <c r="C52" t="s" s="8">
         <v>96</v>
       </c>
-      <c r="D52" s="15"/>
-      <c r="E52" s="15"/>
+      <c r="D52" s="14"/>
+      <c r="E52" s="14"/>
     </row>
     <row r="53" ht="15" customHeight="1">
-      <c r="A53" t="s" s="11">
+      <c r="A53" t="s" s="8">
         <v>3</v>
       </c>
-      <c r="B53" t="s" s="11">
+      <c r="B53" t="s" s="8">
         <v>97</v>
       </c>
-      <c r="C53" t="s" s="12">
+      <c r="C53" t="s" s="11">
         <v>98</v>
       </c>
-      <c r="D53" s="13"/>
-      <c r="E53" s="14"/>
+      <c r="D53" s="12"/>
+      <c r="E53" s="13"/>
     </row>
     <row r="54" ht="15" customHeight="1">
       <c r="A54" t="s" s="8">
@@ -3169,17 +3166,17 @@
       <c r="E55" s="10"/>
     </row>
     <row r="56" ht="15" customHeight="1">
-      <c r="A56" t="s" s="11">
+      <c r="A56" t="s" s="8">
         <v>9</v>
       </c>
-      <c r="B56" t="s" s="11">
+      <c r="B56" t="s" s="8">
         <v>103</v>
       </c>
-      <c r="C56" t="s" s="12">
+      <c r="C56" t="s" s="11">
         <v>104</v>
       </c>
-      <c r="D56" s="13"/>
-      <c r="E56" s="14"/>
+      <c r="D56" s="12"/>
+      <c r="E56" s="13"/>
     </row>
     <row r="57" ht="15" customHeight="1">
       <c r="A57" t="s" s="8">
@@ -3191,21 +3188,21 @@
       <c r="C57" t="s" s="8">
         <v>105</v>
       </c>
-      <c r="D57" s="15"/>
-      <c r="E57" s="15"/>
+      <c r="D57" s="14"/>
+      <c r="E57" s="14"/>
     </row>
     <row r="58" ht="15" customHeight="1">
-      <c r="A58" t="s" s="11">
+      <c r="A58" t="s" s="8">
         <v>9</v>
       </c>
-      <c r="B58" t="s" s="11">
+      <c r="B58" t="s" s="8">
         <v>106</v>
       </c>
-      <c r="C58" t="s" s="12">
+      <c r="C58" t="s" s="11">
         <v>107</v>
       </c>
-      <c r="D58" s="13"/>
-      <c r="E58" s="14"/>
+      <c r="D58" s="12"/>
+      <c r="E58" s="13"/>
     </row>
     <row r="59" ht="15" customHeight="1">
       <c r="A59" t="s" s="8">
@@ -3260,17 +3257,17 @@
       <c r="E62" s="10"/>
     </row>
     <row r="63" ht="15" customHeight="1">
-      <c r="A63" t="s" s="11">
+      <c r="A63" t="s" s="8">
         <v>116</v>
       </c>
-      <c r="B63" t="s" s="11">
+      <c r="B63" t="s" s="8">
         <v>117</v>
       </c>
-      <c r="C63" t="s" s="12">
+      <c r="C63" t="s" s="11">
         <v>118</v>
       </c>
-      <c r="D63" s="13"/>
-      <c r="E63" s="14"/>
+      <c r="D63" s="12"/>
+      <c r="E63" s="13"/>
     </row>
     <row r="64" ht="15" customHeight="1">
       <c r="A64" t="s" s="8">
@@ -3377,17 +3374,17 @@
       <c r="E71" s="10"/>
     </row>
     <row r="72" ht="15" customHeight="1">
-      <c r="A72" t="s" s="11">
+      <c r="A72" t="s" s="8">
         <v>3</v>
       </c>
-      <c r="B72" t="s" s="11">
+      <c r="B72" t="s" s="8">
         <v>133</v>
       </c>
-      <c r="C72" t="s" s="12">
+      <c r="C72" t="s" s="11">
         <v>134</v>
       </c>
-      <c r="D72" s="13"/>
-      <c r="E72" s="14"/>
+      <c r="D72" s="12"/>
+      <c r="E72" s="13"/>
     </row>
     <row r="73" ht="15" customHeight="1">
       <c r="A73" t="s" s="8">
@@ -3598,17 +3595,17 @@
       <c r="E88" s="10"/>
     </row>
     <row r="89" ht="15" customHeight="1">
-      <c r="A89" t="s" s="11">
+      <c r="A89" t="s" s="8">
         <v>9</v>
       </c>
-      <c r="B89" t="s" s="11">
+      <c r="B89" t="s" s="8">
         <v>161</v>
       </c>
-      <c r="C89" t="s" s="12">
+      <c r="C89" t="s" s="11">
         <v>162</v>
       </c>
-      <c r="D89" s="13"/>
-      <c r="E89" s="14"/>
+      <c r="D89" s="12"/>
+      <c r="E89" s="13"/>
     </row>
     <row r="90" ht="15" customHeight="1">
       <c r="A90" t="s" s="8">
@@ -3832,17 +3829,17 @@
       <c r="E106" s="10"/>
     </row>
     <row r="107" ht="15" customHeight="1">
-      <c r="A107" t="s" s="11">
+      <c r="A107" t="s" s="8">
         <v>51</v>
       </c>
-      <c r="B107" t="s" s="11">
+      <c r="B107" t="s" s="8">
         <v>188</v>
       </c>
-      <c r="C107" t="s" s="12">
+      <c r="C107" t="s" s="11">
         <v>189</v>
       </c>
-      <c r="D107" s="13"/>
-      <c r="E107" s="14"/>
+      <c r="D107" s="12"/>
+      <c r="E107" s="13"/>
     </row>
     <row r="108" ht="15" customHeight="1">
       <c r="A108" t="s" s="8">
@@ -3910,17 +3907,17 @@
       <c r="E112" s="10"/>
     </row>
     <row r="113" ht="15" customHeight="1">
-      <c r="A113" t="s" s="11">
+      <c r="A113" t="s" s="8">
         <v>3</v>
       </c>
-      <c r="B113" t="s" s="11">
+      <c r="B113" t="s" s="8">
         <v>199</v>
       </c>
-      <c r="C113" t="s" s="12">
+      <c r="C113" t="s" s="11">
         <v>200</v>
       </c>
-      <c r="D113" s="13"/>
-      <c r="E113" s="14"/>
+      <c r="D113" s="12"/>
+      <c r="E113" s="13"/>
     </row>
     <row r="114" ht="15" customHeight="1">
       <c r="A114" t="s" s="8">
@@ -3976,7 +3973,7 @@
     </row>
     <row r="118" ht="15" customHeight="1">
       <c r="A118" t="s" s="8">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="B118" t="s" s="8">
         <v>208</v>
@@ -4015,7 +4012,7 @@
     </row>
     <row r="121" ht="15" customHeight="1">
       <c r="A121" t="s" s="8">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B121" t="s" s="8">
         <v>214</v>
@@ -4040,17 +4037,17 @@
       <c r="E122" s="10"/>
     </row>
     <row r="123" ht="15" customHeight="1">
-      <c r="A123" t="s" s="11">
+      <c r="A123" t="s" s="8">
         <v>3</v>
       </c>
-      <c r="B123" t="s" s="11">
+      <c r="B123" t="s" s="8">
         <v>218</v>
       </c>
-      <c r="C123" t="s" s="12">
+      <c r="C123" t="s" s="11">
         <v>219</v>
       </c>
-      <c r="D123" s="13"/>
-      <c r="E123" s="14"/>
+      <c r="D123" s="12"/>
+      <c r="E123" s="13"/>
     </row>
     <row r="124" ht="15" customHeight="1">
       <c r="A124" t="s" s="8">
@@ -4092,17 +4089,17 @@
       <c r="E126" s="10"/>
     </row>
     <row r="127" ht="15" customHeight="1">
-      <c r="A127" t="s" s="11">
+      <c r="A127" t="s" s="8">
         <v>6</v>
       </c>
-      <c r="B127" t="s" s="11">
+      <c r="B127" t="s" s="8">
         <v>226</v>
       </c>
-      <c r="C127" t="s" s="12">
+      <c r="C127" t="s" s="11">
         <v>227</v>
       </c>
-      <c r="D127" s="13"/>
-      <c r="E127" s="14"/>
+      <c r="D127" s="12"/>
+      <c r="E127" s="13"/>
     </row>
     <row r="128" ht="15" customHeight="1">
       <c r="A128" t="s" s="8">
@@ -4235,17 +4232,17 @@
       <c r="E137" s="10"/>
     </row>
     <row r="138" ht="15" customHeight="1">
-      <c r="A138" t="s" s="11">
+      <c r="A138" t="s" s="8">
         <v>6</v>
       </c>
-      <c r="B138" t="s" s="11">
+      <c r="B138" t="s" s="8">
         <v>127</v>
       </c>
-      <c r="C138" t="s" s="12">
+      <c r="C138" t="s" s="11">
         <v>247</v>
       </c>
-      <c r="D138" s="13"/>
-      <c r="E138" s="14"/>
+      <c r="D138" s="12"/>
+      <c r="E138" s="13"/>
     </row>
     <row r="139" ht="15" customHeight="1">
       <c r="A139" t="s" s="8">
@@ -4849,12 +4846,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="14.4" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="8.85156" style="16" customWidth="1"/>
-    <col min="2" max="2" width="8.85156" style="16" customWidth="1"/>
-    <col min="3" max="3" width="8.85156" style="16" customWidth="1"/>
-    <col min="4" max="4" width="8.85156" style="16" customWidth="1"/>
-    <col min="5" max="5" width="8.85156" style="16" customWidth="1"/>
-    <col min="6" max="256" width="8.85156" style="16" customWidth="1"/>
+    <col min="1" max="1" width="8.85156" style="15" customWidth="1"/>
+    <col min="2" max="2" width="8.85156" style="15" customWidth="1"/>
+    <col min="3" max="3" width="8.85156" style="15" customWidth="1"/>
+    <col min="4" max="4" width="8.85156" style="15" customWidth="1"/>
+    <col min="5" max="5" width="8.85156" style="15" customWidth="1"/>
+    <col min="6" max="256" width="8.85156" style="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customHeight="1">
@@ -4944,12 +4941,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="14.4" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="52.5" style="17" customWidth="1"/>
-    <col min="2" max="2" width="41.5" style="17" customWidth="1"/>
-    <col min="3" max="3" width="8.85156" style="17" customWidth="1"/>
-    <col min="4" max="4" width="255" style="17" customWidth="1"/>
-    <col min="5" max="5" width="8.85156" style="17" customWidth="1"/>
-    <col min="6" max="256" width="8.85156" style="17" customWidth="1"/>
+    <col min="1" max="1" width="52.5" style="16" customWidth="1"/>
+    <col min="2" max="2" width="41.5" style="16" customWidth="1"/>
+    <col min="3" max="3" width="8.85156" style="16" customWidth="1"/>
+    <col min="4" max="4" width="255" style="16" customWidth="1"/>
+    <col min="5" max="5" width="8.85156" style="16" customWidth="1"/>
+    <col min="6" max="256" width="8.85156" style="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customHeight="1">
@@ -5674,7 +5671,7 @@
     </row>
     <row r="49" ht="15" customHeight="1">
       <c r="A49" t="s" s="8">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B49" t="s" s="8">
         <v>371</v>

</xml_diff>